<commit_message>
CSMIS 1.0 For Demo Showcase
Overall reviewed fixed some bugs
Ready for presentation
</commit_message>
<xml_diff>
--- a/excel_tempFiel.xlsx
+++ b/excel_tempFiel.xlsx
@@ -5,162 +5,78 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CSMIS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CSMIS\Import Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8ED272C0-A784-4956-A9A8-63E39F8E0086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{DD9CDAF3-6808-4359-B952-DDCB314540E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
-    <sheet name="Staff_CSV" sheetId="1" r:id="rId1"/>
+    <sheet name="holiday_CSV" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
-  <si>
-    <t>Sr.</t>
-  </si>
-  <si>
-    <t>Division</t>
-  </si>
-  <si>
-    <t>Staff ID</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>DoorLogNo.</t>
-  </si>
-  <si>
-    <t>Dept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Team </t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>DIV002</t>
-  </si>
-  <si>
-    <t>26-00070</t>
-  </si>
-  <si>
-    <t>Amy Htun</t>
-  </si>
-  <si>
-    <t>Offshore Development Dept-1</t>
-  </si>
-  <si>
-    <t>DOT</t>
-  </si>
-  <si>
-    <t>amyhtun@diracetechnology.com</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>DIV003</t>
-  </si>
-  <si>
-    <t>25-00114</t>
-  </si>
-  <si>
-    <t>Arjun</t>
-  </si>
-  <si>
-    <t>Local Business Dept</t>
-  </si>
-  <si>
-    <t>GGI RPA Development</t>
-  </si>
-  <si>
-    <t>arjun@diracetechnology.com</t>
-  </si>
-  <si>
-    <t>25-00195</t>
-  </si>
-  <si>
-    <t>Aung Chan Myae</t>
-  </si>
-  <si>
-    <t>Common Infrastructure Dept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First Line </t>
-  </si>
-  <si>
-    <t>aungchanmyae@diracetechnology.com</t>
-  </si>
-  <si>
-    <t>25-00220</t>
-  </si>
-  <si>
-    <t>Aung Htet Myet Kyaw</t>
-  </si>
-  <si>
-    <t>FPD(Financial)</t>
-  </si>
-  <si>
-    <t>aunghtetmyetkyaw@diracetechnology.com</t>
-  </si>
-  <si>
-    <t>25-00184</t>
-  </si>
-  <si>
-    <t>Aung Kaung Myat</t>
-  </si>
-  <si>
-    <t>MARK</t>
-  </si>
-  <si>
-    <t>aungkaungmyat@diracetechnology.com</t>
-  </si>
-  <si>
-    <t>25-00055</t>
-  </si>
-  <si>
-    <t>Aung Khant</t>
-  </si>
-  <si>
-    <t>Local Project -1</t>
-  </si>
-  <si>
-    <t>aungkhant@diracetechnology.com</t>
-  </si>
-  <si>
-    <t>25-00119</t>
-  </si>
-  <si>
-    <t>Aung Ko Lin</t>
-  </si>
-  <si>
-    <t>FPD(Securities)</t>
-  </si>
-  <si>
-    <t>aungkolin@diracetechnology.com</t>
-  </si>
-  <si>
-    <t>25-00130</t>
-  </si>
-  <si>
-    <t>Aung Kyaw Myat</t>
-  </si>
-  <si>
-    <t>TDB, D-Base</t>
-  </si>
-  <si>
-    <t>aungkyawmyat@diracetechnology.com</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Holiday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Independence Day	</t>
+  </si>
+  <si>
+    <t>Union Day</t>
+  </si>
+  <si>
+    <t>Peasant’s Day</t>
+  </si>
+  <si>
+    <t>Fullmoon Day of Tabaung</t>
+  </si>
+  <si>
+    <t>Armed Forces Day</t>
+  </si>
+  <si>
+    <t>Thingyan Festival</t>
+  </si>
+  <si>
+    <t>World Worker’s Day</t>
+  </si>
+  <si>
+    <t>Full Moon Day of Kasong</t>
+  </si>
+  <si>
+    <t>Eid Holiday *</t>
+  </si>
+  <si>
+    <t>Martyr’s Day</t>
+  </si>
+  <si>
+    <t>Full Moon Day of Waso</t>
+  </si>
+  <si>
+    <t>Thadingyut Festival</t>
+  </si>
+  <si>
+    <t>Deepavali Holiday *</t>
+  </si>
+  <si>
+    <t>Tazaungdaing Festival</t>
+  </si>
+  <si>
+    <t>National Day</t>
+  </si>
+  <si>
+    <t>Christmas Day</t>
   </si>
 </sst>
 </file>
@@ -644,8 +560,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1001,13 +918,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1017,255 +936,302 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
+      <c r="B2" s="1">
+        <v>44930</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2">
-        <v>40042</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>16</v>
+      <c r="B3" s="1">
+        <v>44969</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3">
-        <v>30075</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>16</v>
+      <c r="B4" s="1">
+        <v>44987</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4">
-        <v>30113</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
+      <c r="B5" s="1">
+        <v>44990</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5">
-        <v>30295</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>9</v>
+      <c r="B6" s="1">
+        <v>45012</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6">
-        <v>30258</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
+      <c r="B7" s="1">
+        <v>45025</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7">
-        <v>40022</v>
-      </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>9</v>
+      <c r="B8" s="1">
+        <v>45026</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8">
-        <v>40045</v>
-      </c>
-      <c r="F8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1">
+        <v>45027</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9">
-        <v>30189</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="B10" s="1">
+        <v>45028</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>45029</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>45030</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="G9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" t="s">
-        <v>46</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="B13" s="1">
+        <v>45031</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>45032</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>45033</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>45047</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>45049</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>45106</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>45126</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>45139</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>45227</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>45228</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>45229</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>45242</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>45256</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>45257</v>
+      </c>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1">
+        <v>45267</v>
+      </c>
+      <c r="C27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1">
+        <v>45285</v>
+      </c>
+      <c r="C28" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>